<commit_message>
Finished thru Question 9/Stuck on INDEX/MATCH only for 9
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ed\Desktop\NSS\NSS_Analytics_Bootcamp_DA_9\Excel Projects\lookups_exercise-edwardbrown750\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C110B53-A2D9-4B6E-8271-68586F63D2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB06C2E8-D200-41A3-A434-EEBFFACAE4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -991,7 +991,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11598369864972524"/>
+          <c:x val="9.1038264332035906E-2"/>
           <c:y val="0.30076443569553807"/>
           <c:w val="0.79297803701823888"/>
           <c:h val="0.61498432487605714"/>
@@ -1049,13 +1049,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20862700</c:v>
+                  <c:v>8609500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22683800</c:v>
+                  <c:v>8925500</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23220300</c:v>
+                  <c:v>8833900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1114,13 +1114,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20036743.4099999</c:v>
+                  <c:v>8499425.3399999905</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21722126.219999898</c:v>
+                  <c:v>8599059.6199999992</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22619057.440000001</c:v>
+                  <c:v>8735843.3100000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1882,16 +1882,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>721518</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>71438</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>783430</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>909637</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>100013</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2218,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5349,7 +5349,7 @@
         <v>24</v>
       </c>
       <c r="G56">
-        <f>VLOOKUP($F56,$A$2:$P$52,MATCH(G$55,$A$1:$P$1,0))</f>
+        <f>VLOOKUP($F56,$A$1:$P$52,MATCH(G$55,$A$1:$P$1,0))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="H56">
@@ -5983,7 +5983,7 @@
         <v>0</v>
       </c>
       <c r="B82" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.45">
@@ -6000,19 +6000,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX(B2:B52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>20862700</v>
+        <v>8609500</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX(C2:C52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>20036743.4099999</v>
-      </c>
-      <c r="E84" t="str" cm="1">
-        <f t="array" ref="E84">_xlfn.XLOOKUP(B$89,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A91,"_rank"),$A$1:$P$1,0)),$A$1:$A$52,FALSE)</f>
-        <v>Clerk and Master - Chancery</v>
-      </c>
-      <c r="F84" cm="1">
-        <f t="array" ref="F84">_xlfn.XLOOKUP(E84,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A91,"_diff_pct"),$A$1:$P$1,0)),FALSE)</f>
-        <v>-0.15235918433091292</v>
+        <v>8499425.3399999905</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.45">
@@ -6021,11 +6013,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX(G2:G52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>22683800</v>
+        <v>8925500</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX(H2:H52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>21722126.219999898</v>
+        <v>8599059.6199999992</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.45">
@@ -6034,11 +6026,11 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX(L2:L52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>23220300</v>
+        <v>8833900</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX(M2:M52,MATCH($B$82,$A$2:$A$52,0))</f>
-        <v>22619057.440000001</v>
+        <v>8735843.3100000005</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.45">
@@ -6086,25 +6078,88 @@
       <c r="A91" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
+      <c r="B91" t="str" cm="1">
+        <f t="array" ref="B91">_xlfn.XLOOKUP($B$89, INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A91,"_rank"), $A$1:$P$1,0)), $A$1:$A$52, FALSE)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C91" s="5" cm="1">
+        <f t="array" ref="C91">_xlfn.XLOOKUP($B91, $A$2:$A$52, INDEX($A$2:$P$52,,MATCH(_xlfn.CONCAT($A91,"_diff_pct"), $A$1:$P$1,0)), FALSE)</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D91" t="str" cm="1">
+        <f t="array" ref="D91">_xlfn.XLOOKUP($D$89, INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A91,"_rank"), $A$1:$P$1,0)), $A$1:$A$52, FALSE)</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E91" s="5" cm="1">
+        <f t="array" ref="E91">_xlfn.XLOOKUP($D91, $A$2:$A$52, INDEX($A$2:$P$52,,MATCH(_xlfn.CONCAT($A91,"_diff_pct"), $A$1:$P$1,0)), FALSE)</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F91" t="str" cm="1">
+        <f t="array" ref="F91">_xlfn.XLOOKUP($F$89, INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A91,"_rank"), $A$1:$P$1,0)), $A$1:$A$52, FALSE)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G91" s="5" cm="1">
+        <f t="array" ref="G91">_xlfn.XLOOKUP($F91, $A$2:$A$52, INDEX($A$2:$P$52,,MATCH(_xlfn.CONCAT($A91,"_diff_pct"), $A$1:$P$1,0)), FALSE)</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="B92" t="str" cm="1">
+        <f t="array" ref="B92">_xlfn.XLOOKUP($B$89, INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A92,"_rank"), $A$1:$P$1,0)), $A$1:$A$52, FALSE)</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C92" s="5" cm="1">
+        <f t="array" ref="C92">_xlfn.XLOOKUP($B92, $A$2:$A$52, INDEX($A$2:$P$52,,MATCH(_xlfn.CONCAT($A92,"_diff_pct"), $A$1:$P$1,0)), FALSE)</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D92" t="str" cm="1">
+        <f t="array" ref="D92">_xlfn.XLOOKUP($D$89, INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A92,"_rank"), $A$1:$P$1,0)), $A$1:$A$52, FALSE)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E92" s="5" cm="1">
+        <f t="array" ref="E92">_xlfn.XLOOKUP($D92, $A$2:$A$52, INDEX($A$2:$P$52,,MATCH(_xlfn.CONCAT($A92,"_diff_pct"), $A$1:$P$1,0)), FALSE)</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F92" t="str" cm="1">
+        <f t="array" ref="F92">_xlfn.XLOOKUP($F$89, INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A92,"_rank"), $A$1:$P$1,0)), $A$1:$A$52, FALSE)</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G92" s="5" cm="1">
+        <f t="array" ref="G92">_xlfn.XLOOKUP($F92, $A$2:$A$52, INDEX($A$2:$P$52,,MATCH(_xlfn.CONCAT($A92,"_diff_pct"), $A$1:$P$1,0)), FALSE)</f>
+        <v>-0.13918241656366656</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
+      <c r="B93" t="str" cm="1">
+        <f t="array" ref="B93">_xlfn.XLOOKUP($B$89, INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A93,"_rank"), $A$1:$P$1,0)), $A$1:$A$52, FALSE)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C93" s="5" cm="1">
+        <f t="array" ref="C93">_xlfn.XLOOKUP($B93, $A$2:$A$52, INDEX($A$2:$P$52,,MATCH(_xlfn.CONCAT($A93,"_diff_pct"), $A$1:$P$1,0)), FALSE)</f>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D93" t="str" cm="1">
+        <f t="array" ref="D93">_xlfn.XLOOKUP($D$89, INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A93,"_rank"), $A$1:$P$1,0)), $A$1:$A$52, FALSE)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E93" s="5" cm="1">
+        <f t="array" ref="E93">_xlfn.XLOOKUP($D93, $A$2:$A$52, INDEX($A$2:$P$52,,MATCH(_xlfn.CONCAT($A93,"_diff_pct"), $A$1:$P$1,0)), FALSE)</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F93" t="str" cm="1">
+        <f t="array" ref="F93">_xlfn.XLOOKUP($F$89, INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A93,"_rank"), $A$1:$P$1,0)), $A$1:$A$52, FALSE)</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G93" s="5" cm="1">
+        <f t="array" ref="G93">_xlfn.XLOOKUP($F93, $A$2:$A$52, INDEX($A$2:$P$52,,MATCH(_xlfn.CONCAT($A93,"_diff_pct"), $A$1:$P$1,0)), FALSE)</f>
+        <v>-0.12882667147667154</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A95" s="7" t="s">

</xml_diff>

<commit_message>
Finished all questions including Challenge
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ed\Desktop\NSS\NSS_Analytics_Bootcamp_DA_9\Excel Projects\lookups_exercise-edwardbrown750\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB06C2E8-D200-41A3-A434-EEBFFACAE4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D68624-72FF-4485-A913-E580D0A1887D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1883,15 +1883,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>71438</xdr:rowOff>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>128588</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>909637</xdr:colOff>
-      <xdr:row>116</xdr:row>
-      <xdr:rowOff>100013</xdr:rowOff>
+      <xdr:colOff>957262</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>157163</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2218,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6206,27 +6206,90 @@
       <c r="A98" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="G98" s="4"/>
+      <c r="B98" t="str">
+        <f>INDEX($A$1:$A$52,MATCH($B$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A98,"_rank"),$A$1:$P$1,0)),0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C98" s="4">
+        <f>INDEX($A$1:$P$52,MATCH($B98, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A98,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D98" t="str">
+        <f>INDEX($A$1:$A$52,MATCH($D$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A98,"_rank"),$A$1:$P$1,0)),0))</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E98" s="5">
+        <f>INDEX($A$1:$P$52,MATCH($D98, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A98,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F98" t="str">
+        <f>INDEX($A$1:$A$52,MATCH($F$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A98,"_rank"),$A$1:$P$1,0)),0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G98" s="5">
+        <f>INDEX($A$1:$P$52,MATCH($F98, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A98,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="G99" s="4"/>
+      <c r="B99" t="str">
+        <f t="shared" ref="B99:B100" si="22">INDEX($A$1:$A$52,MATCH($B$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A99,"_rank"),$A$1:$P$1,0)),0))</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C99" s="4">
+        <f t="shared" ref="C99:C100" si="23">INDEX($A$1:$P$52,MATCH($B99, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" ref="D99:D100" si="24">INDEX($A$1:$A$52,MATCH($D$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A99,"_rank"),$A$1:$P$1,0)),0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E99" s="5">
+        <f t="shared" ref="E99:E100" si="25">INDEX($A$1:$P$52,MATCH($D99, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F99" t="str">
+        <f t="shared" ref="F99:F100" si="26">INDEX($A$1:$A$52,MATCH($F$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A99,"_rank"),$A$1:$P$1,0)),0))</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G99" s="5">
+        <f t="shared" ref="G99:G100" si="27">INDEX($A$1:$P$52,MATCH($F99, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.13918241656366656</v>
+      </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>75</v>
       </c>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="G100" s="4"/>
+      <c r="B100" t="str">
+        <f t="shared" si="22"/>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C100" s="4">
+        <f t="shared" si="23"/>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="24"/>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E100" s="5">
+        <f t="shared" si="25"/>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F100" t="str">
+        <f t="shared" si="26"/>
+        <v>Election Commission</v>
+      </c>
+      <c r="G100" s="5">
+        <f t="shared" si="27"/>
+        <v>-0.12882667147667154</v>
+      </c>
       <c r="I100" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed all questions, including Challenge
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ed\Desktop\NSS\NSS_Analytics_Bootcamp_DA_9\Excel Projects\lookups_exercise-edwardbrown750\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D68624-72FF-4485-A913-E580D0A1887D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE906D7-2C61-42FE-B9D0-2DF58B396C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1882,16 +1882,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>128588</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>957262</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>157163</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>157163</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2218,8 +2218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2423,7 +2423,7 @@
         <v>-4.9327413275443007E-3</v>
       </c>
       <c r="F4">
-        <f t="shared" si="2"/>
+        <f>_xlfn.RANK.EQ(E4, $E$2:$E$52, 1)</f>
         <v>42</v>
       </c>
       <c r="G4">
@@ -5338,7 +5338,7 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f>VLOOKUP(A56, $A$2:$I$52, 9, FALSE)</f>
+        <f>VLOOKUP(A56, A$2:$I$52, 9, FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
@@ -5353,11 +5353,11 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="H56">
-        <f t="shared" ref="H56:I61" si="9">VLOOKUP($F56,$A$2:$P$52,MATCH(H$55,$A$1:$P$1,0))</f>
+        <f>VLOOKUP($F56,$A$1:$P$52,MATCH(H$55,$A$1:$P$1,0))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="I56">
-        <f t="shared" si="9"/>
+        <f>VLOOKUP($F56,$A$1:$P$52,MATCH(I$55,$A$1:$P$1,0))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5366,30 +5366,30 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="10">VLOOKUP(A57,$A$2:$D$52, 4, FALSE)</f>
+        <f t="shared" ref="B57:B61" si="9">VLOOKUP(A57,$A$2:$D$52, 4, FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:C61" si="11">VLOOKUP(A57, $A$2:$I$52, 9, FALSE)</f>
+        <f>VLOOKUP(A57, A$2:$I$52, 9, FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:D61" si="12">VLOOKUP(A57, $A$2:$N$52, 14, FALSE)</f>
+        <f t="shared" ref="D57:D61" si="10">VLOOKUP(A57, $A$2:$N$52, 14, FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
       <c r="F57" t="s">
         <v>25</v>
       </c>
       <c r="G57">
-        <f t="shared" ref="G57:G61" si="13">VLOOKUP($F57,$A$2:$P$52,MATCH(G$55,$A$1:$P$1,0))</f>
+        <f t="shared" ref="G57:I61" si="11">VLOOKUP($F57,$A$1:$P$52,MATCH(G$55,$A$1:$P$1,0))</f>
         <v>0</v>
       </c>
       <c r="H57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5398,30 +5398,30 @@
         <v>32</v>
       </c>
       <c r="B58">
+        <f t="shared" si="9"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C58">
+        <f>VLOOKUP(A58, A$2:$I$52, 9, FALSE)</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D58">
         <f t="shared" si="10"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="F58" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="11"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C58">
+      <c r="H58">
         <f t="shared" si="11"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D58">
-        <f t="shared" si="12"/>
-        <v>-374962.91000000015</v>
-      </c>
-      <c r="F58" t="s">
-        <v>32</v>
-      </c>
-      <c r="G58">
-        <f t="shared" si="13"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="H58">
-        <f t="shared" si="9"/>
-        <v>-189254.06000000006</v>
-      </c>
       <c r="I58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5430,30 +5430,30 @@
         <v>38</v>
       </c>
       <c r="B59">
+        <f t="shared" si="9"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C59">
+        <f>VLOOKUP(A59, A$2:$I$52, 9, FALSE)</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D59">
         <f t="shared" si="10"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="F59" t="s">
+        <v>38</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="11"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C59">
+      <c r="H59">
         <f t="shared" si="11"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D59">
-        <f t="shared" si="12"/>
-        <v>-72.879999999888241</v>
-      </c>
-      <c r="F59" t="s">
-        <v>38</v>
-      </c>
-      <c r="G59">
-        <f t="shared" si="13"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="H59">
-        <f t="shared" si="9"/>
-        <v>-45485.580000000075</v>
-      </c>
       <c r="I59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5462,30 +5462,30 @@
         <v>39</v>
       </c>
       <c r="B60">
+        <f t="shared" si="9"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C60">
+        <f>VLOOKUP(A60, A$2:$I$52, 9, FALSE)</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D60">
         <f t="shared" si="10"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="F60" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="11"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C60">
+      <c r="H60">
         <f t="shared" si="11"/>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="D60">
-        <f t="shared" si="12"/>
-        <v>-1724.9000000000233</v>
-      </c>
-      <c r="F60" t="s">
-        <v>39</v>
-      </c>
-      <c r="G60">
-        <f t="shared" si="13"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="H60">
-        <f t="shared" si="9"/>
-        <v>-8005.7900000010268</v>
-      </c>
       <c r="I60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5494,30 +5494,30 @@
         <v>55</v>
       </c>
       <c r="B61">
+        <f t="shared" si="9"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C61">
+        <f>VLOOKUP(A61, A$2:$I$52, 9, FALSE)</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D61">
         <f t="shared" si="10"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="F61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="11"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C61">
+      <c r="H61">
         <f t="shared" si="11"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D61">
-        <f t="shared" si="12"/>
-        <v>-82077.349999999627</v>
-      </c>
-      <c r="F61" t="s">
-        <v>55</v>
-      </c>
-      <c r="G61">
-        <f t="shared" si="13"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="H61">
-        <f t="shared" si="9"/>
-        <v>-133456.33000001032</v>
-      </c>
       <c r="I61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5592,15 +5592,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="14">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
+        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="15">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
+        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="16">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
+        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
       <c r="F66" t="s">
@@ -5624,15 +5624,15 @@
         <v>32</v>
       </c>
       <c r="B67">
+        <f t="shared" si="12"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="13"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67">
         <f t="shared" si="14"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="C67">
-        <f t="shared" si="15"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="D67">
-        <f t="shared" si="16"/>
         <v>-374962.91000000015</v>
       </c>
       <c r="F67" t="s">
@@ -5656,15 +5656,15 @@
         <v>38</v>
       </c>
       <c r="B68">
+        <f t="shared" si="12"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="13"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68">
         <f t="shared" si="14"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C68">
-        <f t="shared" si="15"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="16"/>
         <v>-72.879999999888241</v>
       </c>
       <c r="F68" t="s">
@@ -5688,15 +5688,15 @@
         <v>39</v>
       </c>
       <c r="B69">
+        <f t="shared" si="12"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="13"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69">
         <f t="shared" si="14"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C69">
-        <f t="shared" si="15"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="D69">
-        <f t="shared" si="16"/>
         <v>-1724.9000000000233</v>
       </c>
       <c r="F69" t="s">
@@ -5720,15 +5720,15 @@
         <v>55</v>
       </c>
       <c r="B70">
+        <f t="shared" si="12"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="13"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D70">
         <f t="shared" si="14"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="C70">
-        <f t="shared" si="15"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="D70">
-        <f t="shared" si="16"/>
         <v>-82077.349999999627</v>
       </c>
       <c r="F70" t="s">
@@ -5801,15 +5801,15 @@
         <v>24</v>
       </c>
       <c r="G74">
-        <f>INDEX($A$2:$P$52,MATCH($F74,$A$2:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <f>INDEX($A$1:$P$52,MATCH($F74,$A$1:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="H74">
-        <f t="shared" ref="H74:I79" si="17">INDEX($A$2:$P$52,MATCH($F74,$A$2:$A$52,0),MATCH(H$73,$A$1:$P$1,0))</f>
+        <f t="shared" ref="H74:I74" si="15">INDEX($A$1:$P$52,MATCH($F74,$A$1:$A$52,0),MATCH(H$73,$A$1:$P$1,0))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="I74">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5818,30 +5818,30 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="18">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="B75:B79" si="16">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="19">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="C75:C79" si="17">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="20">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="D75:D79" si="18">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>-311228.08999999997</v>
       </c>
       <c r="F75" t="s">
         <v>25</v>
       </c>
       <c r="G75">
-        <f t="shared" ref="G75:G79" si="21">INDEX($A$2:$P$52,MATCH($F75,$A$2:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <f t="shared" ref="G75:I79" si="19">INDEX($A$1:$P$52,MATCH($F75,$A$1:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
         <v>0</v>
       </c>
       <c r="H75">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="I75">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5850,30 +5850,30 @@
         <v>32</v>
       </c>
       <c r="B76">
+        <f t="shared" si="16"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="17"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D76">
         <f t="shared" si="18"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="F76" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="19"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C76">
+      <c r="H76">
         <f t="shared" si="19"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D76">
-        <f t="shared" si="20"/>
-        <v>-374962.91000000015</v>
-      </c>
-      <c r="F76" t="s">
-        <v>32</v>
-      </c>
-      <c r="G76">
-        <f t="shared" si="21"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="17"/>
-        <v>-189254.06000000006</v>
-      </c>
       <c r="I76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5882,30 +5882,30 @@
         <v>38</v>
       </c>
       <c r="B77">
+        <f t="shared" si="16"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="17"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
         <f t="shared" si="18"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="F77" t="s">
+        <v>38</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="19"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C77">
+      <c r="H77">
         <f t="shared" si="19"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D77">
-        <f t="shared" si="20"/>
-        <v>-72.879999999888241</v>
-      </c>
-      <c r="F77" t="s">
-        <v>38</v>
-      </c>
-      <c r="G77">
-        <f t="shared" si="21"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="H77">
-        <f t="shared" si="17"/>
-        <v>-45485.580000000075</v>
-      </c>
       <c r="I77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5914,30 +5914,30 @@
         <v>39</v>
       </c>
       <c r="B78">
+        <f t="shared" si="16"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="17"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
         <f t="shared" si="18"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="F78" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="19"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C78">
+      <c r="H78">
         <f t="shared" si="19"/>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="D78">
-        <f t="shared" si="20"/>
-        <v>-1724.9000000000233</v>
-      </c>
-      <c r="F78" t="s">
-        <v>39</v>
-      </c>
-      <c r="G78">
-        <f t="shared" si="21"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="17"/>
-        <v>-8005.7900000010268</v>
-      </c>
       <c r="I78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5946,30 +5946,30 @@
         <v>55</v>
       </c>
       <c r="B79">
+        <f t="shared" si="16"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="17"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
         <f t="shared" si="18"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="F79" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="19"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C79">
+      <c r="H79">
         <f t="shared" si="19"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D79">
-        <f t="shared" si="20"/>
-        <v>-82077.349999999627</v>
-      </c>
-      <c r="F79" t="s">
-        <v>55</v>
-      </c>
-      <c r="G79">
-        <f t="shared" si="21"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="17"/>
-        <v>-133456.33000001032</v>
-      </c>
       <c r="I79">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -6237,27 +6237,27 @@
         <v>74</v>
       </c>
       <c r="B99" t="str">
-        <f t="shared" ref="B99:B100" si="22">INDEX($A$1:$A$52,MATCH($B$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A99,"_rank"),$A$1:$P$1,0)),0))</f>
+        <f t="shared" ref="B99:B100" si="20">INDEX($A$1:$A$52,MATCH($B$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A99,"_rank"),$A$1:$P$1,0)),0))</f>
         <v>Metropolitan Clerk</v>
       </c>
       <c r="C99" s="4">
-        <f t="shared" ref="C99:C100" si="23">INDEX($A$1:$P$52,MATCH($B99, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <f t="shared" ref="C99:C100" si="21">INDEX($A$1:$P$52,MATCH($B99, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
         <v>-0.17551246244575608</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" ref="D99:D100" si="24">INDEX($A$1:$A$52,MATCH($D$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A99,"_rank"),$A$1:$P$1,0)),0))</f>
+        <f t="shared" ref="D99:D100" si="22">INDEX($A$1:$A$52,MATCH($D$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A99,"_rank"),$A$1:$P$1,0)),0))</f>
         <v>Internal Audit</v>
       </c>
       <c r="E99" s="5">
-        <f t="shared" ref="E99:E100" si="25">INDEX($A$1:$P$52,MATCH($D99, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <f t="shared" ref="E99:E100" si="23">INDEX($A$1:$P$52,MATCH($D99, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
         <v>-0.17103239309050916</v>
       </c>
       <c r="F99" t="str">
-        <f t="shared" ref="F99:F100" si="26">INDEX($A$1:$A$52,MATCH($F$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A99,"_rank"),$A$1:$P$1,0)),0))</f>
+        <f t="shared" ref="F99:F100" si="24">INDEX($A$1:$A$52,MATCH($F$96,INDEX($A$1:$P$52,,MATCH(_xlfn.CONCAT($A99,"_rank"),$A$1:$P$1,0)),0))</f>
         <v>Office of Family Safety</v>
       </c>
       <c r="G99" s="5">
-        <f t="shared" ref="G99:G100" si="27">INDEX($A$1:$P$52,MATCH($F99, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <f t="shared" ref="G99:G100" si="25">INDEX($A$1:$P$52,MATCH($F99, $A$1:$A$52,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
         <v>-0.13918241656366656</v>
       </c>
       <c r="I99" s="4"/>
@@ -6267,27 +6267,27 @@
         <v>75</v>
       </c>
       <c r="B100" t="str">
+        <f t="shared" si="20"/>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C100" s="4">
+        <f t="shared" si="21"/>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D100" t="str">
         <f t="shared" si="22"/>
-        <v>Community Oversight Board</v>
-      </c>
-      <c r="C100" s="4">
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E100" s="5">
         <f t="shared" si="23"/>
-        <v>-0.82994157333333329</v>
-      </c>
-      <c r="D100" t="str">
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F100" t="str">
         <f t="shared" si="24"/>
-        <v>Clerk and Master - Chancery</v>
-      </c>
-      <c r="E100" s="5">
+        <v>Election Commission</v>
+      </c>
+      <c r="G100" s="5">
         <f t="shared" si="25"/>
-        <v>-0.15295680364719175</v>
-      </c>
-      <c r="F100" t="str">
-        <f t="shared" si="26"/>
-        <v>Election Commission</v>
-      </c>
-      <c r="G100" s="5">
-        <f t="shared" si="27"/>
         <v>-0.12882667147667154</v>
       </c>
       <c r="I100" s="4"/>

</xml_diff>